<commit_message>
Nhập excel vào kho đến
</commit_message>
<xml_diff>
--- a/src/main/resources/report_templates/ExcelNhapKhoChoSanXuat_PT.xlsx
+++ b/src/main/resources/report_templates/ExcelNhapKhoChoSanXuat_PT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\MeuPro\MeUVipPro\src\main\resources\report_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314CAB1A-F9A0-494D-8AA0-A881519B8DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C651EAE2-5D15-44F8-87C3-D0D1E7FBFC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>PO</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>Số hợp đồng</t>
-  </si>
-  <si>
-    <t>Ngày nhận hàng</t>
   </si>
   <si>
     <t>Số lượng</t>
@@ -524,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B12" activeCellId="1" sqref="C15 B12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -580,31 +577,28 @@
       <c r="C3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>24</v>
+      <c r="H3" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>31</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="L3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -616,25 +610,24 @@
         <v>45570</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="E4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="5">
+      <c r="G4" s="5">
         <v>5</v>
       </c>
+      <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
     </row>
     <row r="5" spans="1:12" s="6" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
@@ -644,25 +637,24 @@
         <v>45571</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="E5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="5">
+      <c r="G5" s="5">
         <v>6</v>
       </c>
+      <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
     </row>
     <row r="6" spans="1:12" s="6" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
@@ -672,25 +664,24 @@
         <v>45572</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="E6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="5">
+      <c r="G6" s="5">
         <v>7</v>
       </c>
+      <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
     </row>
     <row r="7" spans="1:12" s="6" customFormat="1" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
@@ -700,25 +691,24 @@
         <v>45573</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="E7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="5">
+      <c r="G7" s="5">
         <v>8</v>
       </c>
+      <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
     </row>
     <row r="8" spans="1:12" s="6" customFormat="1" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
@@ -728,25 +718,24 @@
         <v>45574</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="E8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="5">
+      <c r="G8" s="5">
         <v>9</v>
       </c>
+      <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
     </row>
     <row r="9" spans="1:12" s="6" customFormat="1" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
@@ -756,25 +745,24 @@
         <v>45575</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="E9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="5">
+      <c r="G9" s="5">
         <v>10</v>
       </c>
+      <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
     </row>
     <row r="10" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>